<commit_message>
Added empty cell check part.
</commit_message>
<xml_diff>
--- a/Output/Finding Results.xlsx
+++ b/Output/Finding Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\Processes\RKM03\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2233E44-75EA-4231-A5E8-400BA6C2B854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67CA826F-417B-4666-B540-9F66B3781E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="7200" yWindow="1440" windowWidth="21600" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{B881FF5B-B762-4804-AE01-F58347836941}"/>
+    <x:workbookView xWindow="7200" yWindow="2130" windowWidth="21600" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{13278269-957F-491C-B4A4-4248723E724C}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>1. başlık formata uygun.</x:t>
   </x:si>
   <x:si>
+    <x:t>5. satır 5. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
     <x:t>2. başlık formata uygun.</x:t>
   </x:si>
   <x:si>
+    <x:t>7. satır 20. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
     <x:t>3. başlık formata uygun.</x:t>
   </x:si>
   <x:si>
+    <x:t>7. satır 21. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
     <x:t>4. başlık formata uygun.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satır 22. sütun hücresi boş.</x:t>
   </x:si>
   <x:si>
     <x:t>5. başlık formata uygun.</x:t>
@@ -470,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{92C79644-E4E0-48B7-958C-73FA9788C3FE}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{5503A3FE-9992-4ACD-8290-755AD8725394}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -480,119 +492,131 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="2" spans="1:1">
+    <x:row r="2" spans="1:2">
       <x:c r="A2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1">
+      <x:c r="B2" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
       <x:c r="A3" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
       <x:c r="A4" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
       <x:c r="A5" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:1">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
       <x:c r="A6" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:1">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
       <x:c r="A7" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:1">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
       <x:c r="A8" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:1">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
       <x:c r="A9" s="1" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:1">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
       <x:c r="A10" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:1">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
       <x:c r="A11" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:1">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
       <x:c r="A12" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:1">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
       <x:c r="A13" s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:1">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
       <x:c r="A14" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:1">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
       <x:c r="A15" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:1">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:2">
       <x:c r="A16" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:1">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:2">
       <x:c r="A17" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:1">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:2">
       <x:c r="A18" s="1" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:1">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:2">
       <x:c r="A19" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:1">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:2">
       <x:c r="A20" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:1">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:2">
       <x:c r="A21" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:1">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:2">
       <x:c r="A22" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:1">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:2">
       <x:c r="A23" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:1">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:2">
       <x:c r="A24" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Header check and emptry cell check parts are complete.
</commit_message>
<xml_diff>
--- a/Output/Finding Results.xlsx
+++ b/Output/Finding Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\Processes\RKM03\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67CA826F-417B-4666-B540-9F66B3781E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{231D8306-0FEA-42E5-BF7E-984D874E3BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="7200" yWindow="2130" windowWidth="21600" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{13278269-957F-491C-B4A4-4248723E724C}"/>
+    <x:workbookView xWindow="7200" yWindow="2130" windowWidth="21600" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{06776B7F-B1D4-4CA2-B613-2EABC3DE2EA0}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,87 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
-    <x:t>1. başlık formata uygun.</x:t>
+    <x:t>7. başlık formata uygun değil.</x:t>
   </x:si>
   <x:si>
     <x:t>5. satır 5. sütun hücresi boş.</x:t>
   </x:si>
   <x:si>
-    <x:t>2. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
     <x:t>7. satır 20. sütun hücresi boş.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3. başlık formata uygun.</x:t>
   </x:si>
   <x:si>
     <x:t>7. satır 21. sütun hücresi boş.</x:t>
   </x:si>
   <x:si>
-    <x:t>4. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
     <x:t>7. satır 22. sütun hücresi boş.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22. başlık formata uygun.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23. başlık formata uygun.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -482,7 +416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{5503A3FE-9992-4ACD-8290-755AD8725394}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{D4B1C877-8543-4569-BCE5-1DF890CE23BE}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -501,122 +435,18 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
-      <x:c r="A3" s="1" t="s">
+      <x:c r="B3" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="1" t="s">
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="B4" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
-      <x:c r="A4" s="1" t="s">
+    <x:row r="5" spans="1:2">
+      <x:c r="B5" s="1" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="B4" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
-      <x:c r="A5" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B5" s="1" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2">
-      <x:c r="A6" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:2">
-      <x:c r="A7" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:2">
-      <x:c r="A8" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:2">
-      <x:c r="A9" s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:2">
-      <x:c r="A10" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2">
-      <x:c r="A11" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:2">
-      <x:c r="A12" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:2">
-      <x:c r="A13" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:2">
-      <x:c r="A14" s="1" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:2">
-      <x:c r="A15" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:2">
-      <x:c r="A16" s="1" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:2">
-      <x:c r="A17" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:2">
-      <x:c r="A18" s="1" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:2">
-      <x:c r="A19" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:2">
-      <x:c r="A20" s="1" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:2">
-      <x:c r="A21" s="1" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:2">
-      <x:c r="A22" s="1" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:2">
-      <x:c r="A23" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:2">
-      <x:c r="A24" s="1" t="s">
-        <x:v>26</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Developing 11th part's first part.
</commit_message>
<xml_diff>
--- a/Output/Finding Results.xlsx
+++ b/Output/Finding Results.xlsx
@@ -1,116 +1,181 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR997437\Desktop\RAS Otomasyon\Processes\RKM03\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3944148-6933-46CC-82B3-FEC7FE00FD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AAF1E40-7D88-4AB5-A66F-37EFFBBBA325}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{1AAF1E40-7D88-4AB5-A66F-37EFFBBBA325}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>5. satır 5. sütun hücresi boş.</t>
-  </si>
-  <si>
-    <t>3. satırdaki kontrol kodu değeri doğru değil: KKR</t>
-  </si>
-  <si>
-    <t>7. satırdaki kontrol numarası değeri doğru değil: 006</t>
-  </si>
-  <si>
-    <t>4. satırdaki değer doğru değil: deneme</t>
-  </si>
-  <si>
-    <t>7. satır 20. sütun hücresi boş.</t>
-  </si>
-  <si>
-    <t>8. satırdaki değer doğru değil: -</t>
-  </si>
-  <si>
-    <t>7. satır 21. sütun hücresi boş.</t>
-  </si>
-  <si>
-    <t>7. satır 22. sütun hücresi boş.</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <x:si>
+    <x:t>5. satır 5. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3. satırdaki kontrol kodu değeri doğru değil: KKR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satırdaki kontrol numarası değeri doğru değil: 006</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4. satırdaki değer doğru değil: deneme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satır 20. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8. satırdaki değer doğru değil: -</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satır 21. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satır 22. sütun hücresi boş.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8. satırdaki popülasyon sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8. satırdaki test için alınan örnek sayısı doğru değil ('?' olmalıydı): Tüm</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:charset val="162"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,54 +474,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50432F00-B441-4ADE-A127-D1D5BB4B0B66}">
-  <dimension ref="B2:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="B2:E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{50432F00-B441-4ADE-A127-D1D5BB4B0B66}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="B2:E5"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E3" sqref="E3 E3:E3 B2:E5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="26.710938" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="44.285156" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="47.570312" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="35.710938" style="2" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="B2" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="B3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="B4" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="B5" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="G6" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="G7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:7">
+      <x:c r="G9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:7">
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="G11" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="G12" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="G13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="G14" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:7">
+      <x:c r="G15" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:7">
+      <x:c r="G16" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:7">
+      <x:c r="G17" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>